<commit_message>
update dsstore for pitagora tools
</commit_message>
<xml_diff>
--- a/tool_development/pipeline_manifest.xlsx
+++ b/tool_development/pipeline_manifest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/biocore01/projects/Biocore/biocore-pipelines/tool_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13D61315-465A-B640-BA34-D684CF6E9FD0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8087733A-BEC5-1943-9736-CC4D6BA5E833}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24000" yWindow="-3780" windowWidth="24000" windowHeight="21340" xr2:uid="{D4C3ED08-622B-0246-89D2-5F67CB6F7F2D}"/>
+    <workbookView xWindow="-24020" yWindow="15440" windowWidth="24000" windowHeight="18720" xr2:uid="{D4C3ED08-622B-0246-89D2-5F67CB6F7F2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>QC SE CLT Components</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Wrapped?</t>
   </si>
@@ -51,6 +48,27 @@
   </si>
   <si>
     <t>Timestamped?</t>
+  </si>
+  <si>
+    <t>01-qc-se.cwl</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Pipeline Component</t>
+  </si>
+  <si>
+    <t>Workflow / CLT?</t>
+  </si>
+  <si>
+    <t>Workflow</t>
+  </si>
+  <si>
+    <t>GGR</t>
   </si>
 </sst>
 </file>
@@ -67,7 +85,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -94,9 +112,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,40 +430,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00EA8326-4843-DA49-8DC3-D50DB9011579}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="32.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="1" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>